<commit_message>
Update individual sim analysis file
</commit_message>
<xml_diff>
--- a/src/inversionInvasionsProject.xlsx
+++ b/src/inversionInvasionsProject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraschaal/Documents/Northeastern/LotterhosLab/Coding/SLiM/CoreSim_QTL/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EF7008-620E-7945-A301-951818675A0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196E0BA5-8BA9-5343-8594-B75D1907E08E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30340" yWindow="960" windowWidth="31300" windowHeight="19220" xr2:uid="{C7F3A2BF-0708-CC46-AFFD-E54380C2BABF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{C7F3A2BF-0708-CC46-AFFD-E54380C2BABF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>Project Deadline</t>
   </si>
@@ -132,12 +132,6 @@
     <t xml:space="preserve">Full Methods Draft </t>
   </si>
   <si>
-    <t>Revisit wish list sims</t>
-  </si>
-  <si>
-    <t>Determine statistics for analyzing data</t>
-  </si>
-  <si>
     <t>1 full day</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>2 weeks</t>
   </si>
   <si>
-    <t>2 hours</t>
-  </si>
-  <si>
     <t>1 week</t>
   </si>
   <si>
@@ -183,9 +174,6 @@
     <t>Final Draft of Methods</t>
   </si>
   <si>
-    <t>Write up statistics for methods</t>
-  </si>
-  <si>
     <t>Full Draft Results</t>
   </si>
   <si>
@@ -232,6 +220,12 @@
   </si>
   <si>
     <t>writing goal intro para 4-6</t>
+  </si>
+  <si>
+    <t>Determine adaptive inversion criteria</t>
+  </si>
+  <si>
+    <t>Write up analysis methods</t>
   </si>
 </sst>
 </file>
@@ -609,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EE9B69-9279-5A46-BA18-DA4D73F2065C}">
-  <dimension ref="A1:Y36"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -629,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -709,7 +703,7 @@
         <v>44246</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -717,27 +711,27 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4">
         <v>44249</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4">
         <v>44255</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -745,384 +739,373 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4">
         <v>44253</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4">
         <v>44265</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4">
-        <v>44257</v>
+        <v>44270</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4">
-        <v>44258</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
+        <v>44265</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4">
-        <v>44260</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
+        <v>44267</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4">
-        <v>44265</v>
-      </c>
-      <c r="G10" t="s">
-        <v>35</v>
+        <v>44271</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4">
-        <v>44267</v>
-      </c>
-      <c r="G11" t="s">
-        <v>35</v>
+        <v>44287</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4">
-        <v>44271</v>
+        <v>44272</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4">
-        <v>44249</v>
+        <v>44281</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
       </c>
       <c r="I13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="4">
-        <v>44272</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
+        <v>44293</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4">
-        <v>44281</v>
-      </c>
-      <c r="H15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
+        <v>44309</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C16" s="4">
-        <v>44309</v>
-      </c>
-      <c r="J16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" t="s">
-        <v>35</v>
-      </c>
-      <c r="L16" t="s">
-        <v>35</v>
+        <v>44313</v>
+      </c>
+      <c r="M16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4">
-        <v>44313</v>
+        <v>44326</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="N17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4">
-        <v>44326</v>
-      </c>
-      <c r="M18" t="s">
+        <v>44340</v>
+      </c>
+      <c r="N18" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
-      </c>
-      <c r="N18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
       </c>
       <c r="C19" s="4">
         <v>44340</v>
       </c>
-      <c r="N19" t="s">
+      <c r="Q19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="O19" t="s">
-        <v>35</v>
-      </c>
-      <c r="P19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
       <c r="C20" s="4">
-        <v>44340</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>35</v>
+        <v>44351</v>
+      </c>
+      <c r="R20" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4">
-        <v>44351</v>
-      </c>
-      <c r="R21" t="s">
-        <v>35</v>
+        <v>44358</v>
+      </c>
+      <c r="S21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C22" s="4">
-        <v>44358</v>
+        <v>44361</v>
       </c>
       <c r="S22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4">
-        <v>44361</v>
-      </c>
-      <c r="S23" t="s">
-        <v>35</v>
+        <v>44372</v>
+      </c>
+      <c r="T23" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" s="4">
-        <v>44372</v>
-      </c>
-      <c r="T24" t="s">
-        <v>35</v>
+        <v>44379</v>
+      </c>
+      <c r="U24" t="s">
+        <v>33</v>
+      </c>
+      <c r="V24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="4">
-        <v>44379</v>
-      </c>
-      <c r="U25" t="s">
-        <v>35</v>
-      </c>
-      <c r="V25" t="s">
-        <v>35</v>
+        <v>44384</v>
+      </c>
+      <c r="W25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C26" s="4">
         <v>44384</v>
       </c>
       <c r="W26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C27" s="4">
-        <v>44384</v>
+        <v>44386</v>
       </c>
       <c r="W27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="4">
-        <v>44386</v>
-      </c>
-      <c r="W28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C28" s="5">
         <v>44389</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="X29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="X28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>